<commit_message>
3.0.4 correct key value of mapmap.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoTypeReferenceKtConstants.xlsx
+++ b/meta/program/BlancoTypeReferenceKtConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoTypeReferenceKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A344853-71A7-0B4E-A51D-8D7A9342B0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A777D5-B173-C246-A84F-5FB71F422942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,11 +228,11 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"3.0.1"</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>"/typereferencekt"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"3.0.4"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1075,7 +1075,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1119,7 +1119,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1386,7 +1386,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>27</v>
@@ -1406,7 +1406,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>29</v>

</xml_diff>